<commit_message>
PowerPoint über Aktuellen stand hinzugefügt und Gantt aktualisiert
</commit_message>
<xml_diff>
--- a/PocketCoachExcel-PDF/Excel_Tabellen/Gantt_ASIII_PocketCoach_WS2021.xlsx
+++ b/PocketCoachExcel-PDF/Excel_Tabellen/Gantt_ASIII_PocketCoach_WS2021.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\$UERI00-RQTSDAVQA0QL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilswagner/Documents/HSHL/Semester_7/Assistenztechnologie_III/AbschlussProjekt_PocketCoach/Git_Struktur_ordner/PocketCoach/PocketCoachExcel-PDF/Excel_Tabellen/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC5FD94-B5F0-8742-8344-7AF3766B07A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplaner" sheetId="1" r:id="rId1"/>
@@ -709,7 +710,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -1743,6 +1744,21 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,24 +1816,9 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="41" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="59">
-    <cellStyle name="% abgeschlossen" xfId="16"/>
+    <cellStyle name="% abgeschlossen" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20 % - Akzent1" xfId="36" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="40" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="44" builtinId="38" customBuiltin="1"/>
@@ -1836,7 +1837,7 @@
     <cellStyle name="60 % - Akzent4" xfId="50" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent5" xfId="54" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60 % - Akzent6" xfId="58" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Aktivität" xfId="2"/>
+    <cellStyle name="Aktivität" xfId="2" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Akzent1" xfId="35" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Akzent2" xfId="39" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Akzent3" xfId="43" builtinId="37" customBuiltin="1"/>
@@ -1845,36 +1846,36 @@
     <cellStyle name="Akzent6" xfId="55" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="28" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="29" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Bezeichnung" xfId="5"/>
+    <cellStyle name="Bezeichnung" xfId="5" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
     <cellStyle name="Dezimal [0]" xfId="20" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Eingabe" xfId="27" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="34" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="24" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Komma" xfId="19" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15"/>
-    <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18"/>
-    <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17"/>
+    <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="15" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="18" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="17" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Neutral" xfId="26" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="33" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Planlegende" xfId="14"/>
-    <cellStyle name="Projektüberschriften" xfId="4"/>
+    <cellStyle name="Planlegende" xfId="14" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Projektüberschriften" xfId="4" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Prozent" xfId="23" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Prozent abgeschlossen" xfId="6"/>
+    <cellStyle name="Prozent abgeschlossen" xfId="6" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Schlecht" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7"/>
+    <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="7" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Überschrift" xfId="8" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Überschrift 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Überschrift 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Überschriften für Zeiträume" xfId="3"/>
+    <cellStyle name="Überschriften für Zeiträume" xfId="3" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Verknüpfte Zelle" xfId="30" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Währung" xfId="21" builtinId="4" customBuiltin="1"/>
     <cellStyle name="Währung [0]" xfId="22" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Warnender Text" xfId="32" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zeitraumwert" xfId="13"/>
+    <cellStyle name="Zeitraumwert" xfId="13" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="Zelle überprüfen" xfId="31" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="240">
@@ -5485,24 +5486,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:ES32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="53.25" style="2" customWidth="1"/>
-    <col min="3" max="4" width="17.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="17.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="3" customWidth="1"/>
     <col min="8" max="27" width="3.5" style="1" customWidth="1"/>
     <col min="28" max="149" width="3.5" customWidth="1"/>
@@ -5512,11 +5513,11 @@
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="58" t="s">
         <v>62</v>
       </c>
@@ -5524,80 +5525,80 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:149" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="62" t="s">
+    <row r="2" spans="2:149" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="16">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="J2" s="8"/>
-      <c r="K2" s="75" t="s">
+      <c r="K2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
       <c r="Q2" s="22"/>
-      <c r="R2" s="75" t="s">
+      <c r="R2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
       <c r="X2" s="23"/>
-      <c r="Y2" s="73" t="s">
+      <c r="Y2" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
-      <c r="AC2" s="74"/>
-      <c r="AD2" s="74"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79"/>
       <c r="AE2" s="24"/>
-      <c r="AF2" s="73" t="s">
+      <c r="AF2" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="74"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="74"/>
-      <c r="AK2" s="74"/>
-      <c r="AL2" s="74"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="74"/>
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="79"/>
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
       <c r="AO2" s="25"/>
-      <c r="AP2" s="73" t="s">
+      <c r="AP2" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="74"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="74"/>
-      <c r="AU2" s="74"/>
-      <c r="AV2" s="74"/>
-      <c r="AW2" s="74"/>
-      <c r="AX2" s="74"/>
-      <c r="AY2" s="74"/>
-      <c r="AZ2" s="74"/>
-      <c r="BA2" s="77"/>
-      <c r="BB2" s="77"/>
-      <c r="BC2" s="77"/>
-      <c r="BD2" s="77"/>
-      <c r="BE2" s="77"/>
+      <c r="AQ2" s="79"/>
+      <c r="AR2" s="79"/>
+      <c r="AS2" s="79"/>
+      <c r="AT2" s="79"/>
+      <c r="AU2" s="79"/>
+      <c r="AV2" s="79"/>
+      <c r="AW2" s="79"/>
+      <c r="AX2" s="79"/>
+      <c r="AY2" s="79"/>
+      <c r="AZ2" s="79"/>
+      <c r="BA2" s="82"/>
+      <c r="BB2" s="82"/>
+      <c r="BC2" s="82"/>
+      <c r="BD2" s="82"/>
+      <c r="BE2" s="82"/>
     </row>
-    <row r="3" spans="2:149" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:149" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>46</v>
       </c>
@@ -5657,7 +5658,7 @@
       <c r="BD3" s="37"/>
       <c r="BE3" s="37"/>
     </row>
-    <row r="4" spans="2:149" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:149" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>44</v>
       </c>
@@ -5717,7 +5718,7 @@
       <c r="BD4" s="37"/>
       <c r="BE4" s="37"/>
     </row>
-    <row r="5" spans="2:149" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:149" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21" t="s">
         <v>45</v>
       </c>
@@ -5770,215 +5771,215 @@
       <c r="AY5" s="14"/>
       <c r="AZ5" s="14"/>
     </row>
-    <row r="6" spans="2:149" s="5" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="63" t="s">
+    <row r="6" spans="2:149" s="5" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="70" t="s">
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="72"/>
-      <c r="V6" s="70" t="s">
+      <c r="P6" s="76"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="W6" s="71"/>
-      <c r="X6" s="71"/>
-      <c r="Y6" s="71"/>
-      <c r="Z6" s="71"/>
-      <c r="AA6" s="71"/>
-      <c r="AB6" s="72"/>
-      <c r="AC6" s="70" t="s">
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="77"/>
+      <c r="AC6" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="AD6" s="71"/>
-      <c r="AE6" s="71"/>
-      <c r="AF6" s="71"/>
-      <c r="AG6" s="71"/>
-      <c r="AH6" s="71"/>
-      <c r="AI6" s="72"/>
-      <c r="AJ6" s="70" t="s">
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="76"/>
+      <c r="AG6" s="76"/>
+      <c r="AH6" s="76"/>
+      <c r="AI6" s="77"/>
+      <c r="AJ6" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="AK6" s="71"/>
-      <c r="AL6" s="71"/>
-      <c r="AM6" s="71"/>
-      <c r="AN6" s="71"/>
-      <c r="AO6" s="71"/>
-      <c r="AP6" s="72"/>
-      <c r="AQ6" s="70" t="s">
+      <c r="AK6" s="76"/>
+      <c r="AL6" s="76"/>
+      <c r="AM6" s="76"/>
+      <c r="AN6" s="76"/>
+      <c r="AO6" s="76"/>
+      <c r="AP6" s="77"/>
+      <c r="AQ6" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="AR6" s="71"/>
-      <c r="AS6" s="71"/>
-      <c r="AT6" s="71"/>
-      <c r="AU6" s="71"/>
-      <c r="AV6" s="71"/>
-      <c r="AW6" s="72"/>
-      <c r="AX6" s="70" t="s">
+      <c r="AR6" s="76"/>
+      <c r="AS6" s="76"/>
+      <c r="AT6" s="76"/>
+      <c r="AU6" s="76"/>
+      <c r="AV6" s="76"/>
+      <c r="AW6" s="77"/>
+      <c r="AX6" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="AY6" s="71"/>
-      <c r="AZ6" s="71"/>
-      <c r="BA6" s="71"/>
-      <c r="BB6" s="71"/>
-      <c r="BC6" s="71"/>
-      <c r="BD6" s="72"/>
-      <c r="BE6" s="70" t="s">
+      <c r="AY6" s="76"/>
+      <c r="AZ6" s="76"/>
+      <c r="BA6" s="76"/>
+      <c r="BB6" s="76"/>
+      <c r="BC6" s="76"/>
+      <c r="BD6" s="77"/>
+      <c r="BE6" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="BF6" s="71"/>
-      <c r="BG6" s="71"/>
-      <c r="BH6" s="71"/>
-      <c r="BI6" s="71"/>
-      <c r="BJ6" s="71"/>
-      <c r="BK6" s="72"/>
-      <c r="BL6" s="70" t="s">
+      <c r="BF6" s="76"/>
+      <c r="BG6" s="76"/>
+      <c r="BH6" s="76"/>
+      <c r="BI6" s="76"/>
+      <c r="BJ6" s="76"/>
+      <c r="BK6" s="77"/>
+      <c r="BL6" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="BM6" s="71"/>
-      <c r="BN6" s="71"/>
-      <c r="BO6" s="71"/>
-      <c r="BP6" s="71"/>
-      <c r="BQ6" s="71"/>
-      <c r="BR6" s="71"/>
-      <c r="BS6" s="72"/>
-      <c r="BT6" s="70" t="s">
+      <c r="BM6" s="76"/>
+      <c r="BN6" s="76"/>
+      <c r="BO6" s="76"/>
+      <c r="BP6" s="76"/>
+      <c r="BQ6" s="76"/>
+      <c r="BR6" s="76"/>
+      <c r="BS6" s="77"/>
+      <c r="BT6" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="BU6" s="71"/>
-      <c r="BV6" s="71"/>
-      <c r="BW6" s="71"/>
-      <c r="BX6" s="71"/>
-      <c r="BY6" s="71"/>
-      <c r="BZ6" s="72"/>
-      <c r="CA6" s="67" t="s">
+      <c r="BU6" s="76"/>
+      <c r="BV6" s="76"/>
+      <c r="BW6" s="76"/>
+      <c r="BX6" s="76"/>
+      <c r="BY6" s="76"/>
+      <c r="BZ6" s="77"/>
+      <c r="CA6" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="CB6" s="68"/>
-      <c r="CC6" s="68"/>
-      <c r="CD6" s="68"/>
-      <c r="CE6" s="68"/>
-      <c r="CF6" s="68"/>
-      <c r="CG6" s="69"/>
-      <c r="CH6" s="70" t="s">
+      <c r="CB6" s="73"/>
+      <c r="CC6" s="73"/>
+      <c r="CD6" s="73"/>
+      <c r="CE6" s="73"/>
+      <c r="CF6" s="73"/>
+      <c r="CG6" s="74"/>
+      <c r="CH6" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="CI6" s="71"/>
-      <c r="CJ6" s="71"/>
-      <c r="CK6" s="71"/>
-      <c r="CL6" s="71"/>
-      <c r="CM6" s="71"/>
-      <c r="CN6" s="72"/>
-      <c r="CO6" s="70" t="s">
+      <c r="CI6" s="76"/>
+      <c r="CJ6" s="76"/>
+      <c r="CK6" s="76"/>
+      <c r="CL6" s="76"/>
+      <c r="CM6" s="76"/>
+      <c r="CN6" s="77"/>
+      <c r="CO6" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="CP6" s="71"/>
-      <c r="CQ6" s="71"/>
-      <c r="CR6" s="71"/>
-      <c r="CS6" s="71"/>
-      <c r="CT6" s="71"/>
-      <c r="CU6" s="72"/>
-      <c r="CV6" s="70" t="s">
+      <c r="CP6" s="76"/>
+      <c r="CQ6" s="76"/>
+      <c r="CR6" s="76"/>
+      <c r="CS6" s="76"/>
+      <c r="CT6" s="76"/>
+      <c r="CU6" s="77"/>
+      <c r="CV6" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="CW6" s="71"/>
-      <c r="CX6" s="71"/>
-      <c r="CY6" s="71"/>
-      <c r="CZ6" s="71"/>
-      <c r="DA6" s="71"/>
-      <c r="DB6" s="72"/>
-      <c r="DC6" s="70" t="s">
+      <c r="CW6" s="76"/>
+      <c r="CX6" s="76"/>
+      <c r="CY6" s="76"/>
+      <c r="CZ6" s="76"/>
+      <c r="DA6" s="76"/>
+      <c r="DB6" s="77"/>
+      <c r="DC6" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="DD6" s="71"/>
-      <c r="DE6" s="71"/>
-      <c r="DF6" s="71"/>
-      <c r="DG6" s="71"/>
-      <c r="DH6" s="71"/>
-      <c r="DI6" s="72"/>
-      <c r="DJ6" s="70" t="s">
+      <c r="DD6" s="76"/>
+      <c r="DE6" s="76"/>
+      <c r="DF6" s="76"/>
+      <c r="DG6" s="76"/>
+      <c r="DH6" s="76"/>
+      <c r="DI6" s="77"/>
+      <c r="DJ6" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="DK6" s="71"/>
-      <c r="DL6" s="71"/>
-      <c r="DM6" s="71"/>
-      <c r="DN6" s="71"/>
-      <c r="DO6" s="71"/>
-      <c r="DP6" s="72"/>
-      <c r="DQ6" s="70" t="s">
+      <c r="DK6" s="76"/>
+      <c r="DL6" s="76"/>
+      <c r="DM6" s="76"/>
+      <c r="DN6" s="76"/>
+      <c r="DO6" s="76"/>
+      <c r="DP6" s="77"/>
+      <c r="DQ6" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="DR6" s="71"/>
-      <c r="DS6" s="71"/>
-      <c r="DT6" s="71"/>
-      <c r="DU6" s="71"/>
-      <c r="DV6" s="71"/>
-      <c r="DW6" s="72"/>
-      <c r="DX6" s="70" t="s">
+      <c r="DR6" s="76"/>
+      <c r="DS6" s="76"/>
+      <c r="DT6" s="76"/>
+      <c r="DU6" s="76"/>
+      <c r="DV6" s="76"/>
+      <c r="DW6" s="77"/>
+      <c r="DX6" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="DY6" s="71"/>
-      <c r="DZ6" s="71"/>
-      <c r="EA6" s="71"/>
-      <c r="EB6" s="71"/>
-      <c r="EC6" s="71"/>
-      <c r="ED6" s="72"/>
-      <c r="EE6" s="70" t="s">
+      <c r="DY6" s="76"/>
+      <c r="DZ6" s="76"/>
+      <c r="EA6" s="76"/>
+      <c r="EB6" s="76"/>
+      <c r="EC6" s="76"/>
+      <c r="ED6" s="77"/>
+      <c r="EE6" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="EF6" s="71"/>
-      <c r="EG6" s="71"/>
-      <c r="EH6" s="71"/>
-      <c r="EI6" s="71"/>
-      <c r="EJ6" s="71"/>
-      <c r="EK6" s="71"/>
-      <c r="EL6" s="72"/>
-      <c r="EM6" s="70" t="s">
+      <c r="EF6" s="76"/>
+      <c r="EG6" s="76"/>
+      <c r="EH6" s="76"/>
+      <c r="EI6" s="76"/>
+      <c r="EJ6" s="76"/>
+      <c r="EK6" s="76"/>
+      <c r="EL6" s="77"/>
+      <c r="EM6" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="EN6" s="71"/>
-      <c r="EO6" s="71"/>
-      <c r="EP6" s="71"/>
-      <c r="EQ6" s="71"/>
-      <c r="ER6" s="71"/>
-      <c r="ES6" s="72"/>
+      <c r="EN6" s="76"/>
+      <c r="EO6" s="76"/>
+      <c r="EP6" s="76"/>
+      <c r="EQ6" s="76"/>
+      <c r="ER6" s="76"/>
+      <c r="ES6" s="77"/>
     </row>
-    <row r="7" spans="2:149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="64"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="61"/>
+    <row r="7" spans="2:149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="69"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="66"/>
       <c r="H7" s="17">
         <v>1</v>
       </c>
@@ -6406,7 +6407,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="40" t="s">
         <v>48</v>
       </c>
@@ -6442,7 +6443,7 @@
       <c r="ER8" s="18"/>
       <c r="ES8" s="56"/>
     </row>
-    <row r="9" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="52" t="s">
         <v>14</v>
       </c>
@@ -6474,7 +6475,7 @@
       <c r="ER9" s="18"/>
       <c r="ES9" s="56"/>
     </row>
-    <row r="10" spans="2:149" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:149" ht="36" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>47</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="45">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="BY10" s="18"/>
       <c r="BZ10" s="1"/>
@@ -6506,7 +6507,7 @@
       <c r="ER10" s="18"/>
       <c r="ES10" s="56"/>
     </row>
-    <row r="11" spans="2:149" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:149" ht="36" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
         <v>49</v>
       </c>
@@ -6523,7 +6524,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="41">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BY11" s="18"/>
       <c r="BZ11" s="1"/>
@@ -6538,7 +6539,7 @@
       <c r="ER11" s="18"/>
       <c r="ES11" s="56"/>
     </row>
-    <row r="12" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="49" t="s">
         <v>15</v>
       </c>
@@ -6555,7 +6556,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="51">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="BY12" s="18"/>
       <c r="BZ12" s="1"/>
@@ -6570,7 +6571,7 @@
       <c r="ER12" s="18"/>
       <c r="ES12" s="56"/>
     </row>
-    <row r="13" spans="2:149" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:149" ht="36" x14ac:dyDescent="0.2">
       <c r="B13" s="42" t="s">
         <v>50</v>
       </c>
@@ -6602,7 +6603,7 @@
       <c r="ER13" s="18"/>
       <c r="ES13" s="56"/>
     </row>
-    <row r="14" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="39" t="s">
         <v>16</v>
       </c>
@@ -6632,7 +6633,7 @@
       <c r="ER14" s="18"/>
       <c r="ES14" s="56"/>
     </row>
-    <row r="15" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="49" t="s">
         <v>17</v>
       </c>
@@ -6662,7 +6663,7 @@
       <c r="ER15" s="18"/>
       <c r="ES15" s="56"/>
     </row>
-    <row r="16" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="39" t="s">
         <v>18</v>
       </c>
@@ -6692,7 +6693,7 @@
       <c r="ER16" s="18"/>
       <c r="ES16" s="56"/>
     </row>
-    <row r="17" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="39" t="s">
         <v>19</v>
       </c>
@@ -6722,7 +6723,7 @@
       <c r="ER17" s="18"/>
       <c r="ES17" s="56"/>
     </row>
-    <row r="18" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="49" t="s">
         <v>20</v>
       </c>
@@ -6752,7 +6753,7 @@
       <c r="ER18" s="18"/>
       <c r="ES18" s="56"/>
     </row>
-    <row r="19" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="42" t="s">
         <v>21</v>
       </c>
@@ -6782,7 +6783,7 @@
       <c r="ER19" s="18"/>
       <c r="ES19" s="56"/>
     </row>
-    <row r="20" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="42" t="s">
         <v>22</v>
       </c>
@@ -6812,7 +6813,7 @@
       <c r="ER20" s="18"/>
       <c r="ES20" s="56"/>
     </row>
-    <row r="21" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="49" t="s">
         <v>23</v>
       </c>
@@ -6842,7 +6843,7 @@
       <c r="ER21" s="18"/>
       <c r="ES21" s="56"/>
     </row>
-    <row r="22" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
         <v>24</v>
       </c>
@@ -6872,7 +6873,7 @@
       <c r="ER22" s="18"/>
       <c r="ES22" s="56"/>
     </row>
-    <row r="23" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="42" t="s">
         <v>25</v>
       </c>
@@ -6902,7 +6903,7 @@
       <c r="ER23" s="18"/>
       <c r="ES23" s="56"/>
     </row>
-    <row r="24" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="49" t="s">
         <v>26</v>
       </c>
@@ -6932,7 +6933,7 @@
       <c r="ER24" s="18"/>
       <c r="ES24" s="56"/>
     </row>
-    <row r="25" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="39" t="s">
         <v>27</v>
       </c>
@@ -6962,7 +6963,7 @@
       <c r="ER25" s="18"/>
       <c r="ES25" s="56"/>
     </row>
-    <row r="26" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="40" t="s">
         <v>28</v>
       </c>
@@ -6992,7 +6993,7 @@
       <c r="ER26" s="18"/>
       <c r="ES26" s="56"/>
     </row>
-    <row r="27" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="49" t="s">
         <v>29</v>
       </c>
@@ -7024,7 +7025,7 @@
       <c r="ER27" s="18"/>
       <c r="ES27" s="56"/>
     </row>
-    <row r="28" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="42" t="s">
         <v>30</v>
       </c>
@@ -7056,7 +7057,7 @@
       <c r="ER28" s="18"/>
       <c r="ES28" s="56"/>
     </row>
-    <row r="29" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="39" t="s">
         <v>31</v>
       </c>
@@ -7085,7 +7086,7 @@
       <c r="ER29" s="18"/>
       <c r="ES29" s="56"/>
     </row>
-    <row r="30" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="49" t="s">
         <v>32</v>
       </c>
@@ -7114,7 +7115,7 @@
       <c r="ER30" s="18"/>
       <c r="ES30" s="56"/>
     </row>
-    <row r="31" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:149" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="40" t="s">
         <v>33</v>
       </c>
@@ -7143,7 +7144,7 @@
       <c r="ER31" s="18"/>
       <c r="ES31" s="56"/>
     </row>
-    <row r="32" spans="2:149" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:149" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BS32" s="1"/>
       <c r="BT32" s="1"/>
       <c r="BU32" s="1"/>
@@ -7998,24 +7999,24 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Projektplaner verwendet Zeiträume für Intervalle. „Start=1“ ist Zeitraum 1 und „Dauer=5“ bedeutet, dass das Projekt von Start bis Ende 5 „Zeiträume“ dauert. Geben Sie ab Zelle B5 Daten ein, um das Diagramm zu aktualisieren." sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Geben Sie einen Wert von 1 bis 60 ein, oder wählen Sie in der Liste einen Zeitraum aus – drücken Sie ABBRECHEN, ALT+NACH-UNTEN und dann die EINGABETASTE, um einen Wert auszuwählen" prompt="Geben Sie einen Zeitraum im Bereich 1 bis 60 ein oder wählen Sie einen Zeitraum aus der Liste aus. Drücken Sie ALT+NACH-UNTEN um in der Liste zu navigieren, und drücken Sie dann EINGABE, um einen Wert auszuwählen." sqref="H2:H5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Projektplaner verwendet Zeiträume für Intervalle. „Start=1“ ist Zeitraum 1 und „Dauer=5“ bedeutet, dass das Projekt von Start bis Ende 5 „Zeiträume“ dauert. Geben Sie ab Zelle B5 Daten ein, um das Diagramm zu aktualisieren." sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Geben Sie einen Wert von 1 bis 60 ein, oder wählen Sie in der Liste einen Zeitraum aus – drücken Sie ABBRECHEN, ALT+NACH-UNTEN und dann die EINGABETASTE, um einen Wert auszuwählen" prompt="Geben Sie einen Zeitraum im Bereich 1 bis 60 ein oder wählen Sie einen Zeitraum aus der Liste aus. Drücken Sie ALT+NACH-UNTEN um in der Liste zu navigieren, und drücken Sie dann EINGABE, um einen Wert auszuwählen." sqref="H2:H5" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="J2:J5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer an" sqref="Q2:Q5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts an" sqref="X2:X5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer über den Plan hinaus an" sqref="AE2:AE5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts über den Plan hinaus an" sqref="AO2:AO5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Zeiträume sind von 1 bis 60 verzeichnet, von Zelle H4 an bis zu Zelle BO4 " sqref="H6 CA6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie Aktivitäten in Spalte B ein, beginnend mit Zelle B5_x000a_" sqref="B6:B7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Startzeitraum des Plans in Spalte C ein, beginnend mit Zelle C5" sqref="C6:C7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die Dauer in Zeiträumen für den Plan in Spalte D ein, beginnend mit Zelle D5" sqref="D6:D7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den tatsächlichen Startzeitraum des Plans in Spalte E ein, beginnend mit Zelle E5" sqref="E6:E7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die tatsächliche Dauer in Zeiträumen für den Plan in Spalte F ein, beginnend mit Zelle F5" sqref="F6:F7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Prozentsatz der Fertigstellung des Projekts in Spalte G ein, beginnend mit Zelle G5" sqref="G6:G7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Projekts. Geben Sie in dieser Zelle einen neuen Titel ein. Heben Sie einen Zeitpunkt in H2 hervor. Die Diagrammlegende befindet sich in den Zeilen J2 bis AI2." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Wählen Sie einen Zeitraum aus, der in H2 hervorgehoben werden soll. Eine Diagrammlegende befindet sich im den Zeilen J2 bis AI2." sqref="BA2:BA4 E5:F5 B5 B2:F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die Dauer des Plans an" sqref="J2:J5" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer an" sqref="Q2:Q5" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts an" sqref="X2:X5" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt die tatsächliche Dauer über den Plan hinaus an" sqref="AE2:AE5" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Diese Legendenzelle gibt den Prozentsatz der Fertigstellung des Projekts über den Plan hinaus an" sqref="AO2:AO5" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Zeiträume sind von 1 bis 60 verzeichnet, von Zelle H4 an bis zu Zelle BO4 " sqref="H6 CA6" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie Aktivitäten in Spalte B ein, beginnend mit Zelle B5_x000a_" sqref="B6:B7" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Startzeitraum des Plans in Spalte C ein, beginnend mit Zelle C5" sqref="C6:C7" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die Dauer in Zeiträumen für den Plan in Spalte D ein, beginnend mit Zelle D5" sqref="D6:D7" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den tatsächlichen Startzeitraum des Plans in Spalte E ein, beginnend mit Zelle E5" sqref="E6:E7" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie die tatsächliche Dauer in Zeiträumen für den Plan in Spalte F ein, beginnend mit Zelle F5" sqref="F6:F7" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Geben Sie den Prozentsatz der Fertigstellung des Projekts in Spalte G ein, beginnend mit Zelle G5" sqref="G6:G7" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Der Titel des Projekts. Geben Sie in dieser Zelle einen neuen Titel ein. Heben Sie einen Zeitpunkt in H2 hervor. Die Diagrammlegende befindet sich in den Zeilen J2 bis AI2." sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Wählen Sie einen Zeitraum aus, der in H2 hervorgehoben werden soll. Eine Diagrammlegende befindet sich im den Zeilen J2 bis AI2." sqref="BA2:BA4 E5:F5 B5 B2:F4" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -8032,23 +8033,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.875" style="78" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" style="59" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="60" t="s">
         <v>64</v>
       </c>
       <c r="B2" t="s">
@@ -8061,71 +8062,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="61" t="s">
         <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="86.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="80" t="s">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="61" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="61" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="60" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="62" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="61" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="82" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="63" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="80" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="61" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>